<commit_message>
Update PM19 Tidsregistrering af Marc.xlsx
update 25/02
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/PM19 Tidsregistrering af Marc.xlsx
+++ b/08 Project Management/Tidsregistrering/PM19 Tidsregistrering af Marc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25498532-77E0-4D81-BAA3-5BEC1D122137}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF234A9E-454B-4052-8252-B083F091DC9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>Dato</t>
   </si>
@@ -163,6 +163,27 @@
   </si>
   <si>
     <t>UT01 - Brugertest af UC01 og UC08</t>
+  </si>
+  <si>
+    <t>UI-prototype android</t>
+  </si>
+  <si>
+    <t>reviewer</t>
+  </si>
+  <si>
+    <t>2 timer</t>
+  </si>
+  <si>
+    <t>10 til 20 min</t>
+  </si>
+  <si>
+    <t>UI-prototype desktop</t>
+  </si>
+  <si>
+    <t>OC0103 - angiv primo</t>
+  </si>
+  <si>
+    <t>1 time</t>
   </si>
 </sst>
 </file>
@@ -313,7 +334,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -354,15 +375,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -745,7 +771,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,7 +780,7 @@
     <col min="3" max="3" width="31.42578125" style="18" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" style="17" customWidth="1"/>
     <col min="5" max="5" width="31" style="17" customWidth="1"/>
-    <col min="6" max="6" width="31" style="22" customWidth="1"/>
+    <col min="6" max="6" width="31" style="21" customWidth="1"/>
     <col min="7" max="7" width="37.28515625" style="6" customWidth="1"/>
     <col min="8" max="8" width="37.28515625" style="2" customWidth="1"/>
   </cols>
@@ -810,8 +836,8 @@
       <c r="E3" s="14">
         <v>0.46875</v>
       </c>
-      <c r="F3" s="20">
-        <v>2</v>
+      <c r="F3" s="25" t="s">
+        <v>44</v>
       </c>
       <c r="G3" s="5">
         <f>E3-D3</f>
@@ -823,275 +849,317 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="21"/>
+      <c r="A4" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="15">
+        <v>43886</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="E4" s="16">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G4" s="5">
         <f t="shared" ref="G4:G32" si="0">E4-D4</f>
-        <v>0</v>
+        <v>6.9444444444444198E-3</v>
       </c>
       <c r="H4" s="1">
         <f>SUM(G$3:G4)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>9.0277777777777735E-2</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="21"/>
+      <c r="A5" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="15">
+        <v>43886</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="E5" s="16">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G5" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9444444444445308E-3</v>
       </c>
       <c r="H5" s="1">
         <f>SUM(G$3:G5)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>9.7222222222222265E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="21"/>
+      <c r="A6" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="15">
+        <v>43886</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>48</v>
+      </c>
       <c r="G6" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.8611111111111049E-2</v>
       </c>
       <c r="H6" s="1">
         <f>SUM(G$3:G6)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
-      <c r="F7" s="21"/>
+      <c r="F7" s="20"/>
       <c r="G7" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(G$3:G7)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
-      <c r="F8" s="21"/>
+      <c r="F8" s="20"/>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H8" s="1">
         <f>SUM(G$3:G8)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
-      <c r="F9" s="21"/>
+      <c r="F9" s="20"/>
       <c r="G9" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H9" s="1">
         <f>SUM(G$3:G9)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
-      <c r="F10" s="21"/>
+      <c r="F10" s="20"/>
       <c r="G10" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H10" s="1">
         <f>SUM(G$3:G10)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C11" s="15"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
-      <c r="F11" s="21"/>
+      <c r="F11" s="20"/>
       <c r="G11" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H11" s="1">
         <f>SUM(G$3:G11)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C12" s="15"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
-      <c r="F12" s="21"/>
+      <c r="F12" s="20"/>
       <c r="G12" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H12" s="1">
         <f>SUM(G$3:G12)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C13" s="15"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
-      <c r="F13" s="21"/>
+      <c r="F13" s="20"/>
       <c r="G13" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H13" s="1">
         <f>SUM(G$3:G13)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C14" s="15"/>
-      <c r="F14" s="21"/>
+      <c r="F14" s="20"/>
       <c r="G14" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H14" s="1">
         <f>SUM(G$3:G14)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C15" s="15"/>
-      <c r="F15" s="21"/>
+      <c r="F15" s="20"/>
       <c r="G15" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H15" s="1">
         <f>SUM(G$3:G15)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C16" s="15"/>
-      <c r="F16" s="21"/>
+      <c r="F16" s="20"/>
       <c r="G16" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H16" s="1">
         <f>SUM(G$3:G16)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="17" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C17" s="15"/>
-      <c r="F17" s="21"/>
+      <c r="F17" s="20"/>
       <c r="G17" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H17" s="1">
         <f>SUM(G$3:G17)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="18" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C18" s="15"/>
-      <c r="F18" s="21"/>
+      <c r="F18" s="20"/>
       <c r="G18" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H18" s="1">
         <f>SUM(G$3:G18)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="19" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C19" s="15"/>
-      <c r="F19" s="21"/>
+      <c r="F19" s="20"/>
       <c r="G19" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H19" s="1">
         <f>SUM(G$3:G19)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C20" s="15"/>
-      <c r="F20" s="21"/>
+      <c r="F20" s="20"/>
       <c r="G20" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H20" s="1">
         <f>SUM(G$3:G20)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="21" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C21" s="15"/>
-      <c r="F21" s="21"/>
+      <c r="F21" s="20"/>
       <c r="G21" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H21" s="1">
         <f>SUM(G$3:G21)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="22" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C22" s="15"/>
-      <c r="F22" s="21"/>
+      <c r="F22" s="20"/>
       <c r="G22" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H22" s="1">
         <f>SUM(G$3:G22)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="23" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C23" s="15"/>
-      <c r="F23" s="21"/>
+      <c r="F23" s="20"/>
       <c r="G23" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H23" s="1">
         <f>SUM(G$3:G23)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="24" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C24" s="15"/>
-      <c r="F24" s="21"/>
+      <c r="F24" s="20"/>
       <c r="G24" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H24" s="1">
         <f>SUM(G$3:G24)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="25" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1102,7 +1170,7 @@
       </c>
       <c r="H25" s="1">
         <f>SUM(G$3:G25)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="26" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1113,7 +1181,7 @@
       </c>
       <c r="H26" s="1">
         <f>SUM(G$3:G26)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="27" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1124,7 +1192,7 @@
       </c>
       <c r="H27" s="1">
         <f>SUM(G$3:G27)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="28" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1135,7 +1203,7 @@
       </c>
       <c r="H28" s="1">
         <f>SUM(G$3:G28)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="29" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1146,7 +1214,7 @@
       </c>
       <c r="H29" s="1">
         <f>SUM(G$3:G29)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="30" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1157,7 +1225,7 @@
       </c>
       <c r="H30" s="1">
         <f>SUM(G$3:G30)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="31" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1168,7 +1236,7 @@
       </c>
       <c r="H31" s="1">
         <f>SUM(G$3:G31)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="32" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1179,7 +1247,7 @@
       </c>
       <c r="H32" s="1">
         <f>SUM(G$3:G32)</f>
-        <v>8.3333333333333315E-2</v>
+        <v>0.14583333333333331</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
@@ -1254,8 +1322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9466DE97-788B-454A-A978-16D65412D85C}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>